<commit_message>
[WBCAMS-480] Update May LMU dataset
</commit_message>
<xml_diff>
--- a/migration/data/WorkBC LMS May_2024.xlsx
+++ b/migration/data/WorkBC LMS May_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CEU\7. WORKBC and PROJECTS\LMI Data Updates\Monthly Labour Force Survey\Drupal\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA6605D-0BCE-47F8-A77B-8E9522E0EB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4E7E7D-7C3E-4EEA-9224-FDBDBCED49FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1742,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2028,7 +2028,7 @@
         <v>-1.7</v>
       </c>
       <c r="C20" s="29">
-        <v>10000</v>
+        <v>-10000</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="36">
@@ -3152,23 +3152,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006256975931115C42B154129ACF64F69B" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6a5bc4137ad5000bb33d4b302e37fb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" xmlns:ns4="6dacf12f-1e0d-46b0-91bd-702888a65233" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b711ee3334e61d74dbc2f1f205886f71" ns3:_="" ns4:_="">
     <xsd:import namespace="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
@@ -3395,10 +3378,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13AD9A7D-2FC8-4FCE-A291-642EFDF647E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDCFECB7-D025-4DEB-B1C9-7FD71B9730FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
+    <ds:schemaRef ds:uri="6dacf12f-1e0d-46b0-91bd-702888a65233"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3421,20 +3432,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDCFECB7-D025-4DEB-B1C9-7FD71B9730FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13AD9A7D-2FC8-4FCE-A291-642EFDF647E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
-    <ds:schemaRef ds:uri="6dacf12f-1e0d-46b0-91bd-702888a65233"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>